<commit_message>
Тест edit catalog, edited Notebook,
</commit_message>
<xml_diff>
--- a/Working_with_form/bin/Debug/Catalog.xlsx
+++ b/Working_with_form/bin/Debug/Catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Категории" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Домашний</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>OficePC2</t>
+  </si>
+  <si>
+    <t>Notebook1</t>
+  </si>
+  <si>
+    <t>Notebook2</t>
+  </si>
+  <si>
+    <t>Notebook3</t>
   </si>
 </sst>
 </file>
@@ -472,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,22 +695,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>132</v>
+      <c r="A1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
       <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>